<commit_message>
1. Minor modifications 2. Added code to generate distance matrix between regions 3. Changed population, area, and location data to each region
</commit_message>
<xml_diff>
--- a/RegionData.xlsx
+++ b/RegionData.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yashtambi/Documents/TUD/Academics/Q2/CH3212_StorageTechnology/MATLAB2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yashtambi/Documents/TUD/Academics/Q2/CH3212_StorageTechnology/Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="69">
   <si>
     <t>Region</t>
   </si>
@@ -229,6 +230,12 @@
   </si>
   <si>
     <t>TotalR4</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Area</t>
   </si>
 </sst>
 </file>
@@ -302,8 +309,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -319,11 +330,15 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -601,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView topLeftCell="A33" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55:E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1658,7 +1673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="150" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -2244,4 +2259,128 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="169" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>23341604</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1873236</v>
+      </c>
+      <c r="D2">
+        <v>46.50462263</v>
+      </c>
+      <c r="E2">
+        <v>-111.1214179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>163777491</v>
+      </c>
+      <c r="C3">
+        <v>1830000</v>
+      </c>
+      <c r="D3">
+        <v>41.437420619047614</v>
+      </c>
+      <c r="E3">
+        <v>-79.231700666666669</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>120634475</v>
+      </c>
+      <c r="C4">
+        <v>2899780</v>
+      </c>
+      <c r="D4">
+        <v>36.372918222222225</v>
+      </c>
+      <c r="E4">
+        <v>-106.97878255555555</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>100416030</v>
+      </c>
+      <c r="C5">
+        <v>1480000</v>
+      </c>
+      <c r="D5">
+        <v>33.986681181818184</v>
+      </c>
+      <c r="E5">
+        <v>-86.403892454545456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>163130331</v>
+      </c>
+      <c r="C6">
+        <v>1964000</v>
+      </c>
+      <c r="D6">
+        <v>22.771809999999999</v>
+      </c>
+      <c r="E6">
+        <v>-102.38692500000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>